<commit_message>
added data driven test for product apis using excel
</commit_message>
<xml_diff>
--- a/testData/UserTestData.xlsx
+++ b/testData/UserTestData.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\athul\eclipse-workspace\InventoryMgmtApiTest\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE54D8E-2A7C-4EAD-9848-FC5D2979EED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9223EF39-99A3-49F1-ABFF-23C914F01D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A4BBE31D-A5C0-49F7-911E-78D5F72AEEAB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{A4BBE31D-A5C0-49F7-911E-78D5F72AEEAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>username</t>
   </si>
@@ -70,13 +72,97 @@
   </si>
   <si>
     <t>testuser1003@hotmail.com</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>sku</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>initialStock</t>
+  </si>
+  <si>
+    <t>currentStock</t>
+  </si>
+  <si>
+    <t>reorderLevel</t>
+  </si>
+  <si>
+    <t>costPrice</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>reservedStock</t>
+  </si>
+  <si>
+    <t>Product1001</t>
+  </si>
+  <si>
+    <t>SKUTEST1001</t>
+  </si>
+  <si>
+    <t>Test Description for Product 1001</t>
+  </si>
+  <si>
+    <t>TestCategory</t>
+  </si>
+  <si>
+    <t>Product1002</t>
+  </si>
+  <si>
+    <t>SKUTEST1002</t>
+  </si>
+  <si>
+    <t>Test Description for Product 1002</t>
+  </si>
+  <si>
+    <t>Product1003</t>
+  </si>
+  <si>
+    <t>SKUTEST1003</t>
+  </si>
+  <si>
+    <t>Test Description for Product 1003</t>
+  </si>
+  <si>
+    <t>SKUTEST#1001</t>
+  </si>
+  <si>
+    <t>SKUTEST#1002</t>
+  </si>
+  <si>
+    <t>SKUTEST#1003</t>
+  </si>
+  <si>
+    <t>Changed Test Description for Product 1001</t>
+  </si>
+  <si>
+    <t>Changed Test Description for Product 1002</t>
+  </si>
+  <si>
+    <t>Changed Test Description for Product 1003</t>
+  </si>
+  <si>
+    <t>TestCategory1</t>
+  </si>
+  <si>
+    <t>TestCategory2</t>
+  </si>
+  <si>
+    <t>TestCategory3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,16 +178,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -109,20 +215,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -142,6 +285,24 @@
     <tableColumn id="1" xr3:uid="{5CBA85B9-77E6-41F2-B165-D313D5CAA298}" name="username"/>
     <tableColumn id="2" xr3:uid="{E3F65266-BF83-44B6-AFCB-CD3A373B7293}" name="email" dataCellStyle="Hyperlink"/>
     <tableColumn id="3" xr3:uid="{6F4B4C6F-84EC-49F7-9CBC-F0E92841DE12}" name="password"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05713C5A-1222-4DD9-BF25-D1E1D52C3118}" name="Table2" displayName="Table2" ref="A1:I4" totalsRowShown="0">
+  <autoFilter ref="A1:I4" xr:uid="{05713C5A-1222-4DD9-BF25-D1E1D52C3118}"/>
+  <tableColumns count="9">
+    <tableColumn id="2" xr3:uid="{5EF6A6E6-62D8-4DFB-84B4-41C7F8DC317C}" name="name"/>
+    <tableColumn id="3" xr3:uid="{DB49E923-2F57-4973-8D3E-89B2F713ABBD}" name="sku"/>
+    <tableColumn id="4" xr3:uid="{70A70A95-8254-4D49-958E-292AE9407A31}" name="description"/>
+    <tableColumn id="5" xr3:uid="{D3871315-272B-4DDC-A158-E4A1D06EAE3D}" name="initialStock"/>
+    <tableColumn id="6" xr3:uid="{BFB6B991-FEE8-4258-B660-878B634469AC}" name="currentStock"/>
+    <tableColumn id="7" xr3:uid="{AF62C61E-5759-4411-9104-1EC52418213D}" name="reorderLevel"/>
+    <tableColumn id="8" xr3:uid="{4092DBA9-4005-4BB0-A93C-12E9154BC4E2}" name="costPrice" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{B1BD0FA9-B331-4AB0-8C63-F6BB9A0088D6}" name="Category"/>
+    <tableColumn id="11" xr3:uid="{6C6CBF49-0CB6-4728-8B46-8A7DDE3F3A26}" name="reservedStock"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -446,7 +607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E02DCAC8-5016-486F-9237-CBA7A11CAB5E}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -512,4 +673,251 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{365A0DDD-15AB-4FEA-8F82-22EA261170F9}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" customWidth="1"/>
+    <col min="8" max="9" width="10.44140625" customWidth="1"/>
+    <col min="10" max="10" width="11.21875" customWidth="1"/>
+    <col min="11" max="11" width="14.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2" s="8">
+        <v>100</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3" s="8">
+        <v>100</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4" s="8">
+        <v>100</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{888DAD05-D496-41E2-9FEB-16EFCE5CA8C1}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="6">
+        <v>15</v>
+      </c>
+      <c r="E2" s="9">
+        <v>120.5</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="7">
+        <v>20</v>
+      </c>
+      <c r="E3" s="10">
+        <v>104.5</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="6">
+        <v>10</v>
+      </c>
+      <c r="E4" s="9">
+        <v>90</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>